<commit_message>
getting the book to compile
</commit_message>
<xml_diff>
--- a/data/excel_table_data.xlsx
+++ b/data/excel_table_data.xlsx
@@ -1,6 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <workbookPr date1904="false"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
   </bookViews>
@@ -12,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="259">
   <si>
     <t>Sepal.Length</t>
   </si>
@@ -735,12 +736,66 @@
   </si>
   <si>
     <t xml:space="preserve">example_table data refreshed on: 2019-06-22 19:03:55</t>
+  </si>
+  <si>
+    <t xml:space="preserve">example_table data refreshed on: 2024-11-22 13:54:40.918951</t>
+  </si>
+  <si>
+    <t xml:space="preserve">example_table data refreshed on: 2024-11-22 13:55:10.304578</t>
+  </si>
+  <si>
+    <t xml:space="preserve">example_table data refreshed on: 2024-11-22 13:55:52.988078</t>
+  </si>
+  <si>
+    <t xml:space="preserve">example_table data refreshed on: 2024-11-22 13:58:57.207118</t>
+  </si>
+  <si>
+    <t xml:space="preserve">example_table data refreshed on: 2024-11-22 14:00:16.26145</t>
+  </si>
+  <si>
+    <t xml:space="preserve">example_table data refreshed on: 2024-11-22 14:02:43.469919</t>
+  </si>
+  <si>
+    <t xml:space="preserve">example_table data refreshed on: 2024-11-22 15:54:40.240006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">example_table data refreshed on: 2024-11-22 16:00:07.42849</t>
+  </si>
+  <si>
+    <t xml:space="preserve">example_table data refreshed on: 2024-11-22 16:01:36.85656</t>
+  </si>
+  <si>
+    <t xml:space="preserve">example_table data refreshed on: 2024-11-22 17:11:24.585274</t>
+  </si>
+  <si>
+    <t xml:space="preserve">example_table data refreshed on: 2024-11-22 17:51:14.991443</t>
+  </si>
+  <si>
+    <t xml:space="preserve">example_table data refreshed on: 2024-11-22 17:53:00.787396</t>
+  </si>
+  <si>
+    <t xml:space="preserve">example_table data refreshed on: 2024-11-22 18:00:28.809238</t>
+  </si>
+  <si>
+    <t xml:space="preserve">example_table data refreshed on: 2024-11-22 18:02:12.152745</t>
+  </si>
+  <si>
+    <t xml:space="preserve">example_table data refreshed on: 2024-11-22 18:07:30.394555</t>
+  </si>
+  <si>
+    <t xml:space="preserve">example_table data refreshed on: 2024-11-22 18:09:12.834294</t>
+  </si>
+  <si>
+    <t xml:space="preserve">example_table data refreshed on: 2024-11-22 18:56:03.33679</t>
+  </si>
+  <si>
+    <t xml:space="preserve">example_table data refreshed on: 2024-11-22 18:57:47.679701</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
   <fonts count="3">
     <font>
@@ -1315,14 +1370,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="true" workbookViewId="0">
       <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
     <col min="2" max="2" width="13.1640625" hidden="0" customWidth="1"/>
     <col min="3" max="3" width="12.83203125" hidden="0" customWidth="1"/>
@@ -1338,7 +1393,7 @@
   <sheetData>
     <row r="5">
       <c r="B5" t="s">
-        <v>240</v>
+        <v>258</v>
       </c>
     </row>
     <row r="10">

</xml_diff>